<commit_message>
sync 12/06/23. Added cases.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data_medication.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data_medication.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="35">
   <si>
     <t xml:space="preserve">case_id</t>
   </si>
@@ -91,6 +91,18 @@
     <t xml:space="preserve">wellbeing</t>
   </si>
   <si>
+    <t xml:space="preserve">med_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supplement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">med_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insulin</t>
+  </si>
+  <si>
     <t xml:space="preserve">SNOOZE</t>
   </si>
   <si>
@@ -100,10 +112,19 @@
     <t xml:space="preserve">autonomy</t>
   </si>
   <si>
+    <t xml:space="preserve">record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">record_and_call_careworker</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACKNOWLEDGE</t>
   </si>
   <si>
     <t xml:space="preserve">acknowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">followup</t>
   </si>
 </sst>
 </file>
@@ -241,10 +262,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -357,10 +378,10 @@
         <v>0</v>
       </c>
       <c r="N2" s="5" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="O2" s="5" t="n">
-        <v>1</v>
+        <v>0.21914</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>21</v>
@@ -374,190 +395,1085 @@
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="G3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="K3" s="0"/>
       <c r="L3" s="0" t="s">
         <v>20</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="5" t="n">
-        <v>0</v>
+        <v>0.78</v>
       </c>
       <c r="O3" s="5" t="n">
-        <v>1</v>
+        <v>0.43828</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5" t="n">
+        <v>0.04451</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5" t="n">
+        <v>-0.46</v>
+      </c>
+      <c r="O9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="5" t="n">
+      <c r="B10" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5" t="n">
         <v>0.46</v>
       </c>
-      <c r="O4" s="6" t="n">
+      <c r="O10" s="6" t="n">
         <v>0.04451</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O11" s="5" t="n">
+        <v>0.21914</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R11" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="N13" s="5" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="O13" s="5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N14" s="5" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="O14" s="5" t="n">
+        <v>0.21914</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="5" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="N15" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O15" s="5" t="n">
+        <v>0.21914</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0"/>
-      <c r="K5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
-      <c r="K6" s="0"/>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0"/>
-      <c r="K7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
-      <c r="K8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
-      <c r="K9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-      <c r="K10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-      <c r="K11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0"/>
-      <c r="K12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="K13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="K14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="K15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="K16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="K17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0"/>
+      <c r="L16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5" t="n">
+        <v>0.04451</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="K18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-      <c r="K19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0"/>
-      <c r="K20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0"/>
-      <c r="K21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0"/>
-      <c r="K22" s="0"/>
+      <c r="L18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O18" s="5" t="n">
+        <v>0.21914</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="5" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="O20" s="5" t="n">
+        <v>0.18277</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N21" s="5" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="O21" s="5" t="n">
+        <v>0.21914</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="5" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="N22" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O22" s="5" t="n">
+        <v>0.21914</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0"/>
@@ -670,6 +1586,30 @@
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0"/>
       <c r="K50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0"/>
+      <c r="K51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0"/>
+      <c r="K52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0"/>
+      <c r="K53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0"/>
+      <c r="K54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0"/>
+      <c r="K55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0"/>
+      <c r="K56" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
sync 19/06/23. Bug fixes. tuning the utility functions.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data_medication.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data_medication.xlsx
@@ -286,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M104" activeCellId="0" sqref="M104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -601,10 +601,10 @@
         <v>18</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>0.28</v>
+        <v>0.5</v>
       </c>
       <c r="O6" s="3" t="n">
         <v>0.08</v>
@@ -709,7 +709,7 @@
         <v>18</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N8" s="3" t="n">
         <v>0.4</v>
@@ -929,10 +929,10 @@
         <v>18</v>
       </c>
       <c r="M12" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>-0.22</v>
+        <v>0.28</v>
       </c>
       <c r="O12" s="3" t="n">
         <v>0.18</v>
@@ -1037,7 +1037,7 @@
         <v>18</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N14" s="3" t="n">
         <v>0.4</v>
@@ -1093,7 +1093,7 @@
         <v>18</v>
       </c>
       <c r="M15" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N15" s="3" t="n">
         <v>-0.4</v>
@@ -1149,7 +1149,7 @@
         <v>18</v>
       </c>
       <c r="M16" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N16" s="3" t="n">
         <v>0.4</v>
@@ -1372,7 +1372,7 @@
         <v>-0.5</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>-0.52</v>
+        <v>-0.02</v>
       </c>
       <c r="O20" s="3" t="n">
         <v>0.25</v>
@@ -1477,7 +1477,7 @@
         <v>18</v>
       </c>
       <c r="M22" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N22" s="3" t="n">
         <v>0.4</v>
@@ -1533,7 +1533,7 @@
         <v>18</v>
       </c>
       <c r="M23" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N23" s="3" t="n">
         <v>-0.4</v>
@@ -1589,7 +1589,7 @@
         <v>18</v>
       </c>
       <c r="M24" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N24" s="3" t="n">
         <v>0.4</v>
@@ -1957,10 +1957,10 @@
         <v>18</v>
       </c>
       <c r="M31" s="0" t="n">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>-0.52</v>
+        <v>-0.02</v>
       </c>
       <c r="O31" s="0" t="n">
         <v>0.16</v>
@@ -2065,7 +2065,7 @@
         <v>18</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N33" s="0" t="n">
         <v>0.78</v>
@@ -2285,10 +2285,10 @@
         <v>18</v>
       </c>
       <c r="M37" s="0" t="n">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="N37" s="0" t="n">
-        <v>-0.72</v>
+        <v>-0.22</v>
       </c>
       <c r="O37" s="0" t="n">
         <v>0.37</v>
@@ -2393,7 +2393,7 @@
         <v>18</v>
       </c>
       <c r="M39" s="0" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N39" s="0" t="n">
         <v>0.78</v>
@@ -2449,7 +2449,7 @@
         <v>18</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N40" s="0" t="n">
         <v>-0.78</v>
@@ -2505,7 +2505,7 @@
         <v>18</v>
       </c>
       <c r="M41" s="0" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N41" s="0" t="n">
         <v>0.78</v>
@@ -2728,7 +2728,7 @@
         <v>-0.5</v>
       </c>
       <c r="N45" s="0" t="n">
-        <v>-0.82</v>
+        <v>-0.32</v>
       </c>
       <c r="O45" s="0" t="n">
         <v>0.5</v>
@@ -2833,7 +2833,7 @@
         <v>18</v>
       </c>
       <c r="M47" s="0" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N47" s="0" t="n">
         <v>0.78</v>
@@ -2889,7 +2889,7 @@
         <v>18</v>
       </c>
       <c r="M48" s="0" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N48" s="0" t="n">
         <v>-0.78</v>
@@ -2945,7 +2945,7 @@
         <v>18</v>
       </c>
       <c r="M49" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N49" s="3" t="n">
         <v>0.78</v>
@@ -3305,10 +3305,10 @@
         <v>18</v>
       </c>
       <c r="M56" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="N56" s="3" t="n">
-        <v>-0.82</v>
+        <v>-0.32</v>
       </c>
       <c r="O56" s="3" t="n">
         <v>0.24</v>
@@ -3411,7 +3411,7 @@
         <v>18</v>
       </c>
       <c r="M58" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N58" s="3" t="n">
         <v>0.92</v>
@@ -3629,10 +3629,10 @@
         <v>18</v>
       </c>
       <c r="M62" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="N62" s="3" t="n">
-        <v>-0.9</v>
+        <v>-0.4</v>
       </c>
       <c r="O62" s="3" t="n">
         <v>0.55</v>
@@ -3735,7 +3735,7 @@
         <v>18</v>
       </c>
       <c r="M64" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N64" s="3" t="n">
         <v>0.92</v>
@@ -3791,7 +3791,7 @@
         <v>18</v>
       </c>
       <c r="M65" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N65" s="3" t="n">
         <v>-0.92</v>
@@ -3847,7 +3847,7 @@
         <v>18</v>
       </c>
       <c r="M66" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N66" s="3" t="n">
         <v>0.92</v>
@@ -4068,7 +4068,7 @@
         <v>-0.5</v>
       </c>
       <c r="N70" s="3" t="n">
-        <v>-0.94</v>
+        <v>-0.44</v>
       </c>
       <c r="O70" s="3" t="n">
         <v>0.75</v>
@@ -4171,7 +4171,7 @@
         <v>18</v>
       </c>
       <c r="M72" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N72" s="3" t="n">
         <v>0.92</v>
@@ -4227,7 +4227,7 @@
         <v>18</v>
       </c>
       <c r="M73" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N73" s="3" t="n">
         <v>-0.92</v>
@@ -4283,7 +4283,7 @@
         <v>18</v>
       </c>
       <c r="M74" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N74" s="3" t="n">
         <v>0.92</v>
@@ -4724,10 +4724,10 @@
         <v>18</v>
       </c>
       <c r="M83" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="N83" s="3" t="n">
-        <v>-0.82</v>
+        <v>-0.32</v>
       </c>
       <c r="O83" s="3" t="n">
         <v>0.34</v>
@@ -4830,7 +4830,7 @@
         <v>18</v>
       </c>
       <c r="M85" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N85" s="3" t="n">
         <v>0.92</v>
@@ -5048,10 +5048,10 @@
         <v>18</v>
       </c>
       <c r="M89" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="N89" s="3" t="n">
-        <v>-0.9</v>
+        <v>-0.4</v>
       </c>
       <c r="O89" s="3" t="n">
         <v>0.37</v>
@@ -5154,7 +5154,7 @@
         <v>18</v>
       </c>
       <c r="M91" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N91" s="3" t="n">
         <v>0.92</v>
@@ -5210,7 +5210,7 @@
         <v>18</v>
       </c>
       <c r="M92" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N92" s="3" t="n">
         <v>-0.92</v>
@@ -5266,7 +5266,7 @@
         <v>18</v>
       </c>
       <c r="M93" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N93" s="3" t="n">
         <v>0.92</v>
@@ -5487,7 +5487,7 @@
         <v>-0.5</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>-0.94</v>
+        <v>-0.44</v>
       </c>
       <c r="O97" s="3" t="n">
         <v>0.4</v>
@@ -5590,7 +5590,7 @@
         <v>18</v>
       </c>
       <c r="M99" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N99" s="3" t="n">
         <v>0.92</v>
@@ -5646,7 +5646,7 @@
         <v>18</v>
       </c>
       <c r="M100" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N100" s="3" t="n">
         <v>-0.92</v>
@@ -5702,7 +5702,7 @@
         <v>18</v>
       </c>
       <c r="M101" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N101" s="3" t="n">
         <v>0.92</v>
@@ -6058,10 +6058,10 @@
         <v>18</v>
       </c>
       <c r="M108" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="N108" s="3" t="n">
-        <v>-0.98</v>
+        <v>-0.48</v>
       </c>
       <c r="O108" s="3" t="n">
         <v>1</v>
@@ -6164,7 +6164,7 @@
         <v>18</v>
       </c>
       <c r="M110" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N110" s="3" t="n">
         <v>0.98</v>
@@ -6382,10 +6382,10 @@
         <v>18</v>
       </c>
       <c r="M114" s="3" t="n">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="N114" s="3" t="n">
-        <v>-0.98</v>
+        <v>-0.48</v>
       </c>
       <c r="O114" s="3" t="n">
         <v>1</v>
@@ -6488,7 +6488,7 @@
         <v>18</v>
       </c>
       <c r="M116" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N116" s="3" t="n">
         <v>0.98</v>
@@ -6544,7 +6544,7 @@
         <v>18</v>
       </c>
       <c r="M117" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N117" s="3" t="n">
         <v>-0.98</v>
@@ -6600,7 +6600,7 @@
         <v>18</v>
       </c>
       <c r="M118" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N118" s="3" t="n">
         <v>0.98</v>
@@ -6821,7 +6821,7 @@
         <v>-0.5</v>
       </c>
       <c r="N122" s="3" t="n">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="O122" s="3" t="n">
         <v>1</v>
@@ -6924,7 +6924,7 @@
         <v>18</v>
       </c>
       <c r="M124" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N124" s="3" t="n">
         <v>0.98</v>
@@ -6980,7 +6980,7 @@
         <v>18</v>
       </c>
       <c r="M125" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="N125" s="3" t="n">
         <v>-0.98</v>
@@ -7036,7 +7036,7 @@
         <v>18</v>
       </c>
       <c r="M126" s="3" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="N126" s="3" t="n">
         <v>0.98</v>

</xml_diff>

<commit_message>
sync 20/06/23. Bug fixes. added new cases.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data_medication.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data_medication.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="35">
   <si>
     <t xml:space="preserve">case_id</t>
   </si>
@@ -284,10 +284,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S128"/>
+  <dimension ref="A1:S153"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M104" activeCellId="0" sqref="M104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S121" activeCellId="0" sqref="S121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7163,6 +7163,1340 @@
         <v>20</v>
       </c>
     </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O129" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P129" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q129" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R129" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E130" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F130" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G130" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H130" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M130" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N130" s="3" t="n">
+        <v>-0.92</v>
+      </c>
+      <c r="O130" s="3" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="P130" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q130" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R130" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E131" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F131" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G131" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H131" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I131" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L131" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O131" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P131" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q131" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R131" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E132" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F132" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G132" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H132" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I132" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J132" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K132" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L132" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P132" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q132" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R132" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E133" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F133" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G133" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H133" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I133" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J133" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L133" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M133" s="3" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="N133" s="3" t="n">
+        <v>-0.44</v>
+      </c>
+      <c r="O133" s="3" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="P133" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q133" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R133" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E134" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F134" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G134" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H134" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I134" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J134" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L134" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M134" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N134" s="3" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="O134" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P134" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q134" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R134" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E135" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F135" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G135" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H135" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I135" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J135" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L135" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M135" s="3" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="N135" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O135" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P135" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q135" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R135" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E136" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F136" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G136" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H136" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I136" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J136" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K136" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L136" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M136" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N136" s="3" t="n">
+        <v>-0.92</v>
+      </c>
+      <c r="O136" s="3" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="P136" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q136" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R136" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E137" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F137" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G137" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H137" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I137" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J137" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L137" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N137" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O137" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P137" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q137" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R137" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E138" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F138" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G138" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H138" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I138" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J138" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K138" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L138" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M138" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O138" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P138" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q138" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R138" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E139" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F139" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G139" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H139" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I139" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J139" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L139" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M139" s="3" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="N139" s="3" t="n">
+        <v>-0.46</v>
+      </c>
+      <c r="O139" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="P139" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q139" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R139" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E140" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F140" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G140" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H140" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I140" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J140" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L140" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M140" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N140" s="3" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="O140" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P140" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q140" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R140" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E141" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F141" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G141" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H141" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I141" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J141" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L141" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M141" s="3" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="N141" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O141" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P141" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q141" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R141" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E142" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F142" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G142" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H142" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I142" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J142" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K142" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L142" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M142" s="3" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="N142" s="3" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="O142" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P142" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q142" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R142" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E143" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F143" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G143" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H143" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I143" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J143" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K143" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L143" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M143" s="3" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="N143" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O143" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P143" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q143" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R143" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E144" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F144" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G144" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H144" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I144" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J144" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K144" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L144" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M144" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N144" s="3" t="n">
+        <v>-0.92</v>
+      </c>
+      <c r="O144" s="3" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="P144" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q144" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R144" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E145" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F145" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G145" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H145" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I145" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J145" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L145" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N145" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O145" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P145" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q145" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R145" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E146" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F146" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G146" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H146" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I146" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J146" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K146" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L146" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M146" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P146" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q146" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R146" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E147" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F147" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G147" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H147" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I147" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J147" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L147" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M147" s="3" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="N147" s="3" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="O147" s="3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P147" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q147" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R147" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E148" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F148" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G148" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H148" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I148" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J148" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L148" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M148" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N148" s="3" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="O148" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P148" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q148" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R148" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E149" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F149" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G149" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H149" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I149" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J149" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L149" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M149" s="3" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="N149" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O149" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P149" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q149" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R149" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E150" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F150" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G150" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H150" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I150" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J150" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K150" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L150" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M150" s="3" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="N150" s="3" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="O150" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P150" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R150" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E151" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F151" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G151" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H151" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I151" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J151" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K151" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L151" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M151" s="3" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="N151" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O151" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P151" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q151" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R151" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E152" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F152" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G152" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H152" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I152" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J152" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K152" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L152" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M152" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N152" s="3" t="n">
+        <v>-0.92</v>
+      </c>
+      <c r="O152" s="3" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="P152" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R152" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E153" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F153" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G153" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H153" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I153" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J153" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L153" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N153" s="3" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="O153" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="P153" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q153" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R153" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>